<commit_message>
Joy Global Presentation Submission
This presentation now includes my electrical points
</commit_message>
<xml_diff>
--- a/Design/Bill of Materials/Bill Of Materials - Updated.xlsx
+++ b/Design/Bill of Materials/Bill Of Materials - Updated.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Desktop\School\Active Classes\Senior Design\Git\AgileRoboticControls\Design\Bill of Materials\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="81">
   <si>
     <t>Name</t>
   </si>
@@ -272,6 +277,15 @@
   </si>
   <si>
     <t>5537T181</t>
+  </si>
+  <si>
+    <t>Ordered</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -311,7 +325,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -347,12 +361,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -376,6 +410,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -386,6 +422,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -434,7 +473,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -469,7 +508,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -678,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,7 +732,7 @@
     <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -709,8 +748,11 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -724,8 +766,11 @@
       <c r="E2" s="2">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -739,8 +784,11 @@
       <c r="E3" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -756,8 +804,11 @@
       <c r="E4" s="2">
         <v>0.59</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -773,8 +824,11 @@
       <c r="E5" s="2">
         <v>6.63</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -790,8 +844,11 @@
       <c r="E6" s="2">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -807,8 +864,11 @@
       <c r="E7" s="2">
         <v>4.1399999999999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -824,8 +884,11 @@
       <c r="E8" s="2">
         <v>8.07</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -839,8 +902,11 @@
       <c r="E9" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -856,8 +922,11 @@
       <c r="E10" s="2">
         <v>27.3</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -873,8 +942,11 @@
       <c r="E11" s="2">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -890,8 +962,11 @@
       <c r="E12" s="2">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
@@ -907,8 +982,11 @@
       <c r="E13" s="2">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
@@ -924,8 +1002,11 @@
       <c r="E14" s="2">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
@@ -941,8 +1022,11 @@
       <c r="E15" s="2">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
@@ -957,6 +1041,9 @@
       </c>
       <c r="E16" s="2">
         <v>0.7</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>